<commit_message>
updates to the paper more index fixes to legend replacement viz update updating abstracts with stats from Dr. Hu
</commit_message>
<xml_diff>
--- a/Tables/Formatted/Statistics Pivot - All Abstracts.xlsx
+++ b/Tables/Formatted/Statistics Pivot - All Abstracts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="1215" yWindow="495" windowWidth="30945" windowHeight="18465"/>
   </bookViews>
   <sheets>
     <sheet name="statistics-pivot" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>1980-1984</t>
   </si>
@@ -84,19 +84,32 @@
     <t>Total p-value</t>
   </si>
   <si>
-    <t>The New England journal of medicine Word Count</t>
-  </si>
-  <si>
-    <t>The New England journal of medicine p-value</t>
+    <t>&lt;.0001</t>
+  </si>
+  <si>
+    <t>NEJM Word Count</t>
+  </si>
+  <si>
+    <t>NEJM p-value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -236,6 +249,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="46">
     <fill>
@@ -419,6 +438,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -489,14 +514,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.749992370372631"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -685,178 +704,144 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="42" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="42" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="43" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="44" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="43" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="45" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="41" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="45" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1192,471 +1177,470 @@
   <dimension ref="B2:N13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" style="3" customWidth="1"/>
-    <col min="5" max="14" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" style="2" customWidth="1"/>
+    <col min="5" max="14" width="10.7109375" style="2" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="26" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="L2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="7">
         <v>88.081999999999994</v>
       </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="D3" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8">
         <v>107.1156</v>
       </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="9">
         <v>97.543499999999995</v>
       </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="H3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="10">
         <v>96.508300000000006</v>
       </c>
-      <c r="J3" s="10">
-        <v>0</v>
+      <c r="J3" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="K3" s="11">
         <v>106.7445</v>
       </c>
-      <c r="L3" s="12">
-        <v>0</v>
-      </c>
-      <c r="M3" s="13">
+      <c r="L3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="12">
         <v>103.5716</v>
       </c>
-      <c r="N3" s="14">
-        <v>0</v>
+      <c r="N3" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="7">
         <v>100.3926</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="D4" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="8">
         <v>109.50749999999999</v>
       </c>
-      <c r="F4" s="6">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="9">
         <v>97.431799999999996</v>
       </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="H4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="10">
         <v>98.797399999999996</v>
       </c>
-      <c r="J4" s="10">
-        <v>0</v>
+      <c r="J4" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="K4" s="11">
         <v>132.94470000000001</v>
       </c>
-      <c r="L4" s="12">
-        <v>0</v>
-      </c>
-      <c r="M4" s="13">
+      <c r="L4" s="24">
+        <v>0.67467158616797096</v>
+      </c>
+      <c r="M4" s="12">
         <v>112.9585</v>
       </c>
-      <c r="N4" s="14">
-        <v>1.09E-2</v>
+      <c r="N4" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="7">
         <v>111.4247</v>
       </c>
-      <c r="D5" s="4">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="D5" s="20">
+        <v>6.9012721961053097E-5</v>
+      </c>
+      <c r="E5" s="8">
         <v>99.884699999999995</v>
       </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="9">
         <v>94.779600000000002</v>
       </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="H5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="10">
         <v>89.751400000000004</v>
       </c>
-      <c r="J5" s="10">
-        <v>0</v>
+      <c r="J5" s="23">
+        <v>1.8882202586912001E-3</v>
       </c>
       <c r="K5" s="11">
         <v>145.34950000000001</v>
       </c>
-      <c r="L5" s="12">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
+      <c r="L5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="12">
         <v>106.0817</v>
       </c>
-      <c r="N5" s="14">
-        <v>0</v>
+      <c r="N5" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="7">
         <v>106.7186</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="D6" s="20">
+        <v>0.69485312639309005</v>
+      </c>
+      <c r="E6" s="8">
         <v>103.1994</v>
       </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="9">
         <v>111.9054</v>
       </c>
-      <c r="H6" s="8">
-        <v>0.24929999999999999</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="H6" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="10">
         <v>80.184700000000007</v>
       </c>
-      <c r="J6" s="10">
-        <v>0</v>
+      <c r="J6" s="23">
+        <v>3.04312758010374E-2</v>
       </c>
       <c r="K6" s="11">
         <v>143.36359999999999</v>
       </c>
-      <c r="L6" s="12">
-        <v>0</v>
-      </c>
-      <c r="M6" s="13">
+      <c r="L6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="12">
         <v>110.5518</v>
       </c>
-      <c r="N6" s="14">
-        <v>0</v>
+      <c r="N6" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="7">
         <v>106.13030000000001</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="D7" s="20">
+        <v>0.48353422493065601</v>
+      </c>
+      <c r="E7" s="8">
         <v>105.59229999999999</v>
       </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="9">
         <v>124.108</v>
       </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="H7" s="22">
+        <v>0.30180057929235299</v>
+      </c>
+      <c r="I7" s="10">
         <v>83.991299999999995</v>
       </c>
-      <c r="J7" s="10">
-        <v>0</v>
+      <c r="J7" s="23">
+        <v>0.58699824383507704</v>
       </c>
       <c r="K7" s="11">
         <v>139.9769</v>
       </c>
-      <c r="L7" s="12">
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
+      <c r="L7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="12">
         <v>113.0214</v>
       </c>
-      <c r="N7" s="14">
-        <v>4.9299999999999997E-2</v>
+      <c r="N7" s="25">
+        <v>1.43274975539155E-3</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="7">
         <v>107.6825</v>
       </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="D8" s="20">
+        <v>0.50700587862639801</v>
+      </c>
+      <c r="E8" s="8">
         <v>122.93989999999999</v>
       </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="9">
         <v>125.3152</v>
       </c>
-      <c r="H8" s="8">
-        <v>1E-4</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="H8" s="22">
+        <v>0.30180057929235299</v>
+      </c>
+      <c r="I8" s="10">
         <v>81.994399999999999</v>
       </c>
-      <c r="J8" s="10">
-        <v>0</v>
+      <c r="J8" s="23">
+        <v>3.1079772182507698E-2</v>
       </c>
       <c r="K8" s="11">
         <v>135.92359999999999</v>
       </c>
-      <c r="L8" s="12">
-        <v>0</v>
-      </c>
-      <c r="M8" s="13">
+      <c r="L8" s="24">
+        <v>6.7583321947595795E-4</v>
+      </c>
+      <c r="M8" s="12">
         <v>116.5839</v>
       </c>
-      <c r="N8" s="14">
-        <v>3.7699999999999997E-2</v>
+      <c r="N8" s="25">
+        <v>5.0975166129875502E-2</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="7">
         <v>110.29689999999999</v>
       </c>
-      <c r="D9" s="4">
-        <v>1.9E-3</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="D9" s="20">
+        <v>8.7588231095236599E-4</v>
+      </c>
+      <c r="E9" s="8">
         <v>126.8061</v>
       </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="9">
         <v>133.56880000000001</v>
       </c>
-      <c r="H9" s="8">
-        <v>0</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="H9" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="10">
         <v>78.892099999999999</v>
       </c>
-      <c r="J9" s="10">
-        <v>0</v>
+      <c r="J9" s="23">
+        <v>6.5933614290025796E-5</v>
       </c>
       <c r="K9" s="11">
         <v>131.63239999999999</v>
       </c>
-      <c r="L9" s="12">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="M9" s="13">
+      <c r="L9" s="24">
+        <v>0.72299912730059801</v>
+      </c>
+      <c r="M9" s="12">
         <v>118.23260000000001</v>
       </c>
-      <c r="N9" s="14">
-        <v>2.0000000000000001E-4</v>
+      <c r="N9" s="25">
+        <v>6.2855123065435901E-5</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="7">
         <v>112.3807</v>
       </c>
-      <c r="D10" s="4">
-        <v>0.33689999999999998</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="8">
         <v>126.8819</v>
       </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="9">
         <v>163.56299999999999</v>
       </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
+      <c r="H10" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="10">
         <v>77.813299999999998</v>
       </c>
-      <c r="J10" s="10">
-        <v>0</v>
+      <c r="J10" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="K10" s="11">
         <v>130.87270000000001</v>
       </c>
-      <c r="L10" s="12">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="M10" s="13">
+      <c r="L10" s="24">
+        <v>0.97116821670613496</v>
+      </c>
+      <c r="M10" s="12">
         <v>128.721</v>
       </c>
-      <c r="N10" s="14">
-        <v>0</v>
+      <c r="N10" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="7">
         <v>120.491</v>
       </c>
-      <c r="D11" s="4">
-        <v>4.7399999999999998E-2</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="D11" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="8">
         <v>120.9068</v>
       </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="9">
         <v>166.6216</v>
       </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
+      <c r="H11" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="10">
         <v>79.2744</v>
       </c>
-      <c r="J11" s="10">
-        <v>0</v>
+      <c r="J11" s="23">
+        <v>8.5220079865786999E-4</v>
       </c>
       <c r="K11" s="11">
         <v>112.5758</v>
       </c>
-      <c r="L11" s="12">
-        <v>0.79569999999999996</v>
-      </c>
-      <c r="M11" s="13">
+      <c r="L11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="12">
         <v>127.1812</v>
       </c>
-      <c r="N11" s="14">
-        <v>0</v>
+      <c r="N11" s="25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="13">
         <v>107.9735</v>
       </c>
-      <c r="D12" s="15">
-        <v>0</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="D12" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="14">
         <v>114.63809999999999</v>
       </c>
-      <c r="F12" s="17">
-        <v>0.84630000000000005</v>
-      </c>
-      <c r="G12" s="18">
+      <c r="F12" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="15">
         <v>120.5771</v>
       </c>
-      <c r="H12" s="19">
-        <v>0</v>
-      </c>
-      <c r="I12" s="20">
+      <c r="H12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="16">
         <v>86.060699999999997</v>
       </c>
-      <c r="J12" s="21">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22">
+      <c r="J12" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="17">
         <v>128.7432</v>
       </c>
-      <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="24">
+      <c r="L12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="18">
         <v>114.7115</v>
       </c>
-      <c r="N12" s="25">
-        <v>1</v>
-      </c>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>